<commit_message>
Mur 1 2 3 4 + prefabs
</commit_message>
<xml_diff>
--- a/Docs/Level design.xlsx
+++ b/Docs/Level design.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikael\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tentapoulpe\Desktop\TetrisLike\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>mur1</t>
   </si>
@@ -129,12 +129,21 @@
   </si>
   <si>
     <t>Choisir bonne piece</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Colonne5</t>
+  </si>
+  <si>
+    <t>animation qui tourne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,7 +182,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -203,13 +215,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:D24" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A2:D24"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Colonne1" dataDxfId="4"/>
-    <tableColumn id="2" name="Colonne2" dataDxfId="3"/>
-    <tableColumn id="3" name="Colonne3" dataDxfId="2"/>
-    <tableColumn id="4" name="Colonne4" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A2:E24" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Colonne2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Colonne3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Colonne4" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B59EE582-82EA-45A9-8ED7-948C61677F91}" name="Colonne5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -511,20 +524,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="1" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -537,8 +550,11 @@
       <c r="D2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -551,14 +567,16 @@
       <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,8 +589,11 @@
       <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -585,8 +606,11 @@
       <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -599,8 +623,11 @@
       <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -611,8 +638,11 @@
         <v>2</v>
       </c>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -623,8 +653,9 @@
         <v>3</v>
       </c>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -635,8 +666,9 @@
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -649,8 +681,9 @@
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -661,8 +694,9 @@
         <v>4</v>
       </c>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -673,8 +707,9 @@
         <v>2</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -687,8 +722,9 @@
       <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -699,8 +735,9 @@
         <v>4</v>
       </c>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -711,8 +748,9 @@
         <v>4</v>
       </c>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -723,8 +761,9 @@
         <v>2</v>
       </c>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -737,8 +776,9 @@
       <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -751,8 +791,9 @@
       <c r="D19" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -765,8 +806,9 @@
       <c r="D20" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -779,8 +821,9 @@
       <c r="D21" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -793,8 +836,9 @@
       <c r="D22" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -807,18 +851,22 @@
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1">
-        <v>10</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mur 15 (en cours)
</commit_message>
<xml_diff>
--- a/Docs/Level design.xlsx
+++ b/Docs/Level design.xlsx
@@ -128,16 +128,16 @@
     <t>tres difficile à placer</t>
   </si>
   <si>
-    <t>Choisir bonne piece</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
     <t>Colonne5</t>
   </si>
   <si>
-    <t>animation qui tourne</t>
+    <t>Choisir la bonne pièce</t>
+  </si>
+  <si>
+    <t>Pixel art</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -590,7 +590,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -607,7 +607,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -624,7 +624,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -639,7 +639,7 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -755,7 +755,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -783,28 +783,28 @@
         <v>13</v>
       </c>
       <c r="B19" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -813,7 +813,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
MUR 15 ET MUR 16 OK
</commit_message>
<xml_diff>
--- a/Docs/Level design.xlsx
+++ b/Docs/Level design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>mur1</t>
   </si>
@@ -528,7 +528,7 @@
   <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,7 +806,9 @@
       <c r="D20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">

</xml_diff>

<commit_message>
Mur 5 6 7 8
</commit_message>
<xml_diff>
--- a/Docs/Level design.xlsx
+++ b/Docs/Level design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>mur1</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>Pixel art</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Colonne6</t>
+  </si>
+  <si>
+    <t>Extré</t>
+  </si>
+  <si>
+    <t>Choix</t>
+  </si>
+  <si>
+    <t>Mindfuck</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Boss pixel art</t>
   </si>
 </sst>
 </file>
@@ -182,7 +200,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -215,14 +236,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A2:E24" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Colonne2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Colonne3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Colonne4" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{B59EE582-82EA-45A9-8ED7-948C61677F91}" name="Colonne5" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A2:F24" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A2:F24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Colonne2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Colonne3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Colonne4" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{B59EE582-82EA-45A9-8ED7-948C61677F91}" name="Colonne5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{9A1C47C6-DBB1-47A8-BFF9-5F539B2B58D3}" name="Colonne6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -525,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E24"/>
+  <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +559,7 @@
     <col min="4" max="4" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -553,8 +575,11 @@
       <c r="E2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -568,15 +593,17 @@
         <v>23</v>
       </c>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,8 +619,11 @@
       <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -609,8 +639,11 @@
       <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -626,8 +659,11 @@
       <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -641,8 +677,11 @@
       <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -653,22 +692,32 @@
         <v>3</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -681,35 +730,54 @@
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -722,35 +790,46 @@
       <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -761,24 +840,34 @@
         <v>2</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -792,8 +881,11 @@
       <c r="E19" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -809,8 +901,11 @@
       <c r="E20" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -824,8 +919,11 @@
         <v>25</v>
       </c>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -839,8 +937,11 @@
         <v>25</v>
       </c>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -854,8 +955,11 @@
         <v>33</v>
       </c>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -869,6 +973,7 @@
         <v>37</v>
       </c>
       <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MUR 9 17 18
</commit_message>
<xml_diff>
--- a/Docs/Level design.xlsx
+++ b/Docs/Level design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>mur1</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Difficile à placer</t>
   </si>
   <si>
-    <t>tres difficile à placer</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -156,6 +153,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Boss pixel art</t>
+  </si>
+  <si>
+    <t>choix minfuck extremités</t>
+  </si>
+  <si>
+    <t>Colonne7</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -236,15 +242,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A2:F24" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A2:F24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Colonne2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Colonne3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Colonne4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{B59EE582-82EA-45A9-8ED7-948C61677F91}" name="Colonne5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{9A1C47C6-DBB1-47A8-BFF9-5F539B2B58D3}" name="Colonne6" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A2:G24" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A2:G24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Colonne2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Colonne3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Colonne4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{B59EE582-82EA-45A9-8ED7-948C61677F91}" name="Colonne5" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{9A1C47C6-DBB1-47A8-BFF9-5F539B2B58D3}" name="Colonne6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{69DA8D6C-8BEE-442C-99D8-53BE01B903C1}" name="Colonne7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -547,19 +554,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="53.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -573,13 +581,16 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -594,16 +605,18 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,13 +630,14 @@
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -637,13 +651,14 @@
         <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -657,13 +672,14 @@
         <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -675,13 +691,14 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -693,13 +710,14 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -711,13 +729,14 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -731,13 +750,14 @@
         <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -751,13 +771,14 @@
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -771,13 +792,14 @@
         <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -791,13 +813,14 @@
         <v>31</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -808,12 +831,15 @@
         <v>1</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -824,12 +850,15 @@
         <v>2</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -841,13 +870,14 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -861,13 +891,14 @@
         <v>32</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -879,13 +910,14 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -896,70 +928,80 @@
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F21" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F22" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -970,10 +1012,11 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>